<commit_message>
Excel Util to read and write data + Extent Report adaptor for creating reports each run
</commit_message>
<xml_diff>
--- a/OutputFile/Output_Results.xlsx
+++ b/OutputFile/Output_Results.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IMDB" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="BOB" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="24">
   <si>
     <t>Average Time Duration of Top 5 Tiles</t>
   </si>
@@ -34,6 +34,60 @@
   </si>
   <si>
     <t>8.94</t>
+  </si>
+  <si>
+    <t>FDRateOfInterest</t>
+  </si>
+  <si>
+    <t>FDMaturityValue</t>
+  </si>
+  <si>
+    <t>FDAmount</t>
+  </si>
+  <si>
+    <t>FDTenure</t>
+  </si>
+  <si>
+    <t>FDMaturityDate</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>5 Years: 0 Months : 0 Days</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>FDTenureDays</t>
+  </si>
+  <si>
+    <t>1826</t>
+  </si>
+  <si>
+    <t>7 Mar 2029</t>
+  </si>
+  <si>
+    <t>AggregateInterestAmount</t>
+  </si>
+  <si>
+    <t>InterestPerQuarter</t>
+  </si>
+  <si>
+    <t>FDDepositType</t>
+  </si>
+  <si>
+    <t>Quarterly Payout</t>
+  </si>
+  <si>
+    <t>1,625</t>
+  </si>
+  <si>
+    <t>₹32,500</t>
+  </si>
+  <si>
+    <t>8 Mar 2029</t>
   </si>
 </sst>
 </file>
@@ -369,7 +423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -395,7 +449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s" s="0">
         <v>4</v>
       </c>
@@ -414,12 +468,340 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="5" customWidth="true" width="16.0"/>
+    <col min="6" max="6" customWidth="true" width="20.0"/>
+    <col min="7" max="7" customWidth="true" width="18.140625"/>
+    <col min="8" max="8" customWidth="true" width="23.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Pushing all assignment work did for BDD automation
</commit_message>
<xml_diff>
--- a/OutputFile/Output_Results.xlsx
+++ b/OutputFile/Output_Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="36">
   <si>
     <t>Average Time Duration of Top 5 Tiles</t>
   </si>
@@ -88,6 +88,42 @@
   </si>
   <si>
     <t>8 Mar 2029</t>
+  </si>
+  <si>
+    <t>Reinvestment (Cumulative)</t>
+  </si>
+  <si>
+    <t>14 Mar 2029</t>
+  </si>
+  <si>
+    <t>138,042</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>2 Years: 11 Months: 0 Days</t>
+  </si>
+  <si>
+    <t>1067</t>
+  </si>
+  <si>
+    <t>7.25</t>
+  </si>
+  <si>
+    <t>14 Feb 2027</t>
+  </si>
+  <si>
+    <t>61,661</t>
+  </si>
+  <si>
+    <t>18 Mar 2029</t>
+  </si>
+  <si>
+    <t>18 Feb 2027</t>
+  </si>
+  <si>
+    <t>17 Apr 2029</t>
   </si>
 </sst>
 </file>
@@ -421,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -460,6 +496,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -468,7 +515,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
@@ -801,6 +848,1512 @@
         <v>21</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G14" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G15" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I16" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H18" s="0"/>
+      <c r="I18" s="0"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E19" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F19" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G19" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I19" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G20" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H20" s="0"/>
+      <c r="I20" s="0"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G21" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H22" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I22" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G23" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H23" s="0"/>
+      <c r="I23" s="0"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E24" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F24" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="G24" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H24" s="0"/>
+      <c r="I24" s="0"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G25" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H25" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I25" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C26" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E26" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C27" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G27" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F28" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G28" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I28" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G29" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E30" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F30" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G30" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C31" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F31" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G31" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I31" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C32" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E32" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G32" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G33" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H33" s="0"/>
+      <c r="I33" s="0"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C34" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G34" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H34" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I34" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F35" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G35" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E36" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G36" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H36" s="0"/>
+      <c r="I36" s="0"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F37" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G37" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H37" s="0"/>
+      <c r="I37" s="0"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E38" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F38" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G38" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H38" s="0"/>
+      <c r="I38" s="0"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C39" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E39" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G39" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H39" s="0"/>
+      <c r="I39" s="0"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C40" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E40" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G40" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H40" s="0"/>
+      <c r="I40" s="0"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C41" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E41" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F41" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G41" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H41" s="0"/>
+      <c r="I41" s="0"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C42" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E42" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G42" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H42" s="0"/>
+      <c r="I42" s="0"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C43" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E43" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F43" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G43" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H43" s="0"/>
+      <c r="I43" s="0"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C44" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E44" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F44" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G44" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H44" s="0"/>
+      <c r="I44" s="0"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E45" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F45" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G45" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H45" s="0"/>
+      <c r="I45" s="0"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C46" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E46" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F46" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G46" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I46" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C47" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E47" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F47" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G47" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H47" s="0"/>
+      <c r="I47" s="0"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C48" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E48" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F48" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G48" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H48" s="0"/>
+      <c r="I48" s="0"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F49" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G49" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H49" s="0"/>
+      <c r="I49" s="0"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F50" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G50" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H50" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I50" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F51" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G51" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H51" s="0"/>
+      <c r="I51" s="0"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E52" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F52" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G52" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H52" s="0"/>
+      <c r="I52" s="0"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C53" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E53" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F53" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G53" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I53" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B54" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C54" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E54" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F54" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G54" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H54" s="0"/>
+      <c r="I54" s="0"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E55" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F55" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G55" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H55" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I55" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E56" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F56" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G56" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H56" s="0"/>
+      <c r="I56" s="0"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E57" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F57" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G57" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H57" s="0"/>
+      <c r="I57" s="0"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D58" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E58" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F58" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G58" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H58" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I58" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D59" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E59" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F59" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G59" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H59" s="0"/>
+      <c r="I59" s="0"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D60" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E60" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F60" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G60" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H60" s="0"/>
+      <c r="I60" s="0"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D61" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E61" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F61" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G61" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H61" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I61" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D62" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E62" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F62" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G62" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H62" s="0"/>
+      <c r="I62" s="0"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B63" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D63" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E63" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F63" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="G63" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="H63" s="0"/>
+      <c r="I63" s="0"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E64" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F64" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G64" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="H64" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I64" t="s" s="0">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D65" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E65" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F65" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G65" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H65" s="0"/>
+      <c r="I65" s="0"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D66" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E66" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F66" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G66" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H66" s="0"/>
+      <c r="I66" s="0"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B67" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C67" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E67" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F67" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="G67" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H67" s="0"/>
+      <c r="I67" s="0"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B68" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C68" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E68" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F68" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="G68" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H68" s="0"/>
+      <c r="I68" s="0"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B69" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C69" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D69" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E69" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="F69" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="G69" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H69" s="0"/>
+      <c r="I69" s="0"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>